<commit_message>
Modfied Specification "User Management", Swagger source codes, and SQL file.
</commit_message>
<xml_diff>
--- a/01_document/04_ソフトウェア実装プロセス/01_ソフトウェア要件定義/05_ユーザー管理.xlsx
+++ b/01_document/04_ソフトウェア実装プロセス/01_ソフトウェア要件定義/05_ユーザー管理.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
@@ -2322,22 +2322,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ID(英数字20文字以内)(改定A-26)</t>
-    <rPh sb="3" eb="6">
-      <t>エイスウジ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>モジ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>イナイ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>カイテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>(改定A-27)</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2632,11 +2616,18 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>ID(改定A-26)</t>
+    <rPh sb="3" eb="5">
+      <t>カイテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2924,6 +2915,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2956,18 +2959,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3341,7 +3332,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3381,7 +3372,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
@@ -3395,7 +3386,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3443,7 +3434,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
@@ -3648,7 +3639,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B23" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
@@ -3750,11 +3741,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3859,7 +3850,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>61</v>
@@ -4102,10 +4093,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B37" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
+        <v>204</v>
+      </c>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
@@ -4357,7 +4348,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4405,34 +4396,34 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="46" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="46"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="42"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="81" x14ac:dyDescent="0.15">
@@ -4476,7 +4467,7 @@
         <v>132</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="54" x14ac:dyDescent="0.15">
@@ -4554,7 +4545,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A80" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
@@ -4574,10 +4565,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -4589,7 +4580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
@@ -4618,10 +4609,10 @@
       <c r="E2" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="G2" s="50"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B3" s="25"/>
@@ -4800,23 +4791,23 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="B13" s="51" t="s">
-        <v>197</v>
+      <c r="B13" s="40" t="s">
+        <v>196</v>
       </c>
       <c r="C13" s="25">
         <v>1</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E13" s="30">
         <v>42926</v>
       </c>
       <c r="F13" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="G13" s="29" t="s">
         <v>199</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="81" x14ac:dyDescent="0.15">
@@ -4825,54 +4816,54 @@
         <v>2</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E14" s="30">
         <v>42926</v>
       </c>
       <c r="F14" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="G14" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="G14" s="29" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="15" spans="2:7" ht="81" x14ac:dyDescent="0.15">
-      <c r="B15" s="52"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="25">
         <v>3</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E15" s="30">
         <v>42926</v>
       </c>
       <c r="F15" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="G15" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="G15" s="29" t="s">
-        <v>204</v>
-      </c>
     </row>
     <row r="16" spans="2:7" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="B16" s="54" t="s">
-        <v>208</v>
+      <c r="B16" s="43" t="s">
+        <v>207</v>
       </c>
       <c r="C16" s="25">
         <v>1</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E16" s="30">
         <v>42935</v>
       </c>
       <c r="F16" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="G16" s="29" t="s">
         <v>210</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>